<commit_message>
V4.12.1.40 - Changes to stationery (KSDK changes - USB library changes)
</commit_message>
<xml_diff>
--- a/PackageFiles/Stationery/Packages/400.Kinetis_SDK/KSDK Matrix.xlsx
+++ b/PackageFiles/Stationery/Packages/400.Kinetis_SDK/KSDK Matrix.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7488" windowWidth="25920" windowHeight="13128"/>
+    <workbookView xWindow="0" yWindow="7490" windowWidth="25920" windowHeight="13130"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="182">
   <si>
     <t>3. ADC Low Power</t>
   </si>
@@ -559,6 +559,24 @@
   </si>
   <si>
     <t>KSDK-usb-with-rtos</t>
+  </si>
+  <si>
+    <t>usbDeviceName</t>
+  </si>
+  <si>
+    <t>usbHostName</t>
+  </si>
+  <si>
+    <t>usbOtgName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;!-- Name of USB device mode header file directory - Enables USB device library --&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;!-- Name of USB host mode header file directory - Enables USB host library --&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;!-- Name of USB OTG mode header file directory - Enables USB otg library --&gt;</t>
   </si>
 </sst>
 </file>
@@ -1015,33 +1033,33 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ99"/>
+  <dimension ref="A1:AJ101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E40" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
-      <selection pane="bottomRight" activeCell="O30" sqref="O30"/>
+      <selection pane="bottomRight" activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.21875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="37.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.77734375" style="3" customWidth="1"/>
-    <col min="5" max="12" width="4.44140625" style="2" customWidth="1"/>
-    <col min="13" max="14" width="4.44140625" style="6" customWidth="1"/>
-    <col min="15" max="36" width="4.44140625" style="2" customWidth="1"/>
-    <col min="37" max="16384" width="8.44140625" style="2"/>
+    <col min="1" max="1" width="35.1796875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="37.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.81640625" style="3" customWidth="1"/>
+    <col min="5" max="12" width="4.453125" style="2" customWidth="1"/>
+    <col min="13" max="14" width="4.453125" style="6" customWidth="1"/>
+    <col min="15" max="36" width="4.453125" style="2" customWidth="1"/>
+    <col min="37" max="16384" width="8.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="5" customFormat="1" ht="98.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" s="5" customFormat="1" ht="100.5" x14ac:dyDescent="0.35">
       <c r="A1" s="14"/>
       <c r="C1" s="10"/>
       <c r="D1" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>69</v>
@@ -1140,7 +1158,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="2">
@@ -1272,13 +1290,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="11" t="str">
         <f>"&lt;!-- These constant enables demos for "&amp;INDEX($E$1:$AJ$1,$D$1)&amp;" --&gt;"</f>
-        <v>&lt;!-- These constant enables demos for frdmkl25z --&gt;</v>
+        <v>&lt;!-- These constant enables demos for frdmk22f --&gt;</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
@@ -1348,7 +1366,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>77</v>
       </c>
@@ -1442,7 +1460,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>45</v>
       </c>
@@ -1451,7 +1469,7 @@
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="29"/>
-        <v>&lt;constant id="demo.KSDK-adc-pdb-trigger" value="false" /&gt;</v>
+        <v>&lt;constant id="demo.KSDK-adc-pdb-trigger" value="true" /&gt;</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>16</v>
@@ -1519,7 +1537,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>46</v>
       </c>
@@ -1604,7 +1622,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>47</v>
       </c>
@@ -1659,7 +1677,7 @@
       <c r="AI7" s="9"/>
       <c r="AJ7" s="9"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>78</v>
       </c>
@@ -1747,7 +1765,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>141</v>
       </c>
@@ -1794,7 +1812,7 @@
       <c r="AI9" s="9"/>
       <c r="AJ9" s="9"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>79</v>
       </c>
@@ -1844,7 +1862,7 @@
       <c r="AI10" s="9"/>
       <c r="AJ10" s="9"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>80</v>
       </c>
@@ -1932,7 +1950,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>81</v>
       </c>
@@ -2026,7 +2044,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>83</v>
       </c>
@@ -2120,7 +2138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>84</v>
       </c>
@@ -2214,7 +2232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>85</v>
       </c>
@@ -2308,7 +2326,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>86</v>
       </c>
@@ -2390,7 +2408,7 @@
       <c r="AI16" s="9"/>
       <c r="AJ16" s="9"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>87</v>
       </c>
@@ -2466,7 +2484,7 @@
       <c r="AI17" s="9"/>
       <c r="AJ17" s="9"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>89</v>
       </c>
@@ -2522,7 +2540,7 @@
       <c r="AI18" s="9"/>
       <c r="AJ18" s="9"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>90</v>
       </c>
@@ -2578,7 +2596,7 @@
       <c r="AI19" s="9"/>
       <c r="AJ19" s="9"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>91</v>
       </c>
@@ -2634,7 +2652,7 @@
       <c r="AI20" s="9"/>
       <c r="AJ20" s="9"/>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>92</v>
       </c>
@@ -2690,7 +2708,7 @@
       <c r="AI21" s="9"/>
       <c r="AJ21" s="9"/>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>93</v>
       </c>
@@ -2746,7 +2764,7 @@
       <c r="AI22" s="9"/>
       <c r="AJ22" s="9"/>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>94</v>
       </c>
@@ -2802,7 +2820,7 @@
       <c r="AI23" s="9"/>
       <c r="AJ23" s="9"/>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>95</v>
       </c>
@@ -2858,7 +2876,7 @@
       <c r="AI24" s="9"/>
       <c r="AJ24" s="9"/>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>96</v>
       </c>
@@ -2914,7 +2932,7 @@
       <c r="AI25" s="9"/>
       <c r="AJ25" s="9"/>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>97</v>
       </c>
@@ -2994,7 +3012,7 @@
       <c r="AI26" s="9"/>
       <c r="AJ26" s="9"/>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>98</v>
       </c>
@@ -3070,7 +3088,7 @@
       <c r="AI27" s="9"/>
       <c r="AJ27" s="9"/>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>99</v>
       </c>
@@ -3082,7 +3100,7 @@
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="29"/>
-        <v>&lt;constant id="demo.KSDK-rtc-function-demo" value="false" /&gt;</v>
+        <v>&lt;constant id="demo.KSDK-rtc-function-demo" value="true" /&gt;</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>16</v>
@@ -3146,7 +3164,7 @@
       <c r="AI28" s="9"/>
       <c r="AJ28" s="9"/>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>100</v>
       </c>
@@ -3204,7 +3222,7 @@
       <c r="AI29" s="9"/>
       <c r="AJ29" s="9"/>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>101</v>
       </c>
@@ -3216,7 +3234,7 @@
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="29"/>
-        <v>&lt;constant id="demo.KSDK-watchdog-timer-reset-demo" value="false" /&gt;</v>
+        <v>&lt;constant id="demo.KSDK-watchdog-timer-reset-demo" value="true" /&gt;</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>16</v>
@@ -3282,13 +3300,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.35">
       <c r="C31" s="3" t="s">
         <v>175</v>
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" si="29"/>
-        <v>&lt;constant id="demo.KSDK-usb-with-rtos" value="false" /&gt;</v>
+        <v>&lt;constant id="demo.KSDK-usb-with-rtos" value="true" /&gt;</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>16</v>
@@ -3325,7 +3343,7 @@
       <c r="AI31" s="9"/>
       <c r="AJ31" s="9"/>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.35">
       <c r="C32" s="3" t="s">
         <v>145</v>
       </c>
@@ -3392,7 +3410,7 @@
       <c r="AI32" s="9"/>
       <c r="AJ32" s="9"/>
     </row>
-    <row r="33" spans="3:36" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C33" s="3" t="s">
         <v>146</v>
       </c>
@@ -3459,7 +3477,7 @@
       <c r="AI33" s="9"/>
       <c r="AJ33" s="9"/>
     </row>
-    <row r="34" spans="3:36" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C34" s="3" t="s">
         <v>147</v>
       </c>
@@ -3526,7 +3544,7 @@
       <c r="AI34" s="9"/>
       <c r="AJ34" s="9"/>
     </row>
-    <row r="35" spans="3:36" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C35" s="3" t="s">
         <v>148</v>
       </c>
@@ -3593,7 +3611,7 @@
       <c r="AI35" s="9"/>
       <c r="AJ35" s="9"/>
     </row>
-    <row r="36" spans="3:36" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C36" s="3" t="s">
         <v>149</v>
       </c>
@@ -3660,13 +3678,13 @@
       <c r="AI36" s="9"/>
       <c r="AJ36" s="9"/>
     </row>
-    <row r="37" spans="3:36" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C37" s="3" t="s">
         <v>150</v>
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" si="29"/>
-        <v>&lt;constant id="demo.KSDK-usb-msd" value="false" /&gt;</v>
+        <v>&lt;constant id="demo.KSDK-usb-msd" value="true" /&gt;</v>
       </c>
       <c r="G37" s="12" t="s">
         <v>69</v>
@@ -3717,7 +3735,7 @@
       <c r="AI37" s="9"/>
       <c r="AJ37" s="9"/>
     </row>
-    <row r="38" spans="3:36" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C38" s="3" t="s">
         <v>151</v>
       </c>
@@ -3784,13 +3802,13 @@
       <c r="AI38" s="9"/>
       <c r="AJ38" s="9"/>
     </row>
-    <row r="39" spans="3:36" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C39" s="3" t="s">
         <v>159</v>
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" si="29"/>
-        <v>&lt;constant id="demo.KSDK-usb-host-audio-speaker" value="false" /&gt;</v>
+        <v>&lt;constant id="demo.KSDK-usb-host-audio-speaker" value="true" /&gt;</v>
       </c>
       <c r="G39" s="12" t="s">
         <v>69</v>
@@ -3843,13 +3861,13 @@
       <c r="AI39" s="9"/>
       <c r="AJ39" s="9"/>
     </row>
-    <row r="40" spans="3:36" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C40" s="3" t="s">
         <v>152</v>
       </c>
       <c r="D40" s="3" t="str">
         <f t="shared" si="29"/>
-        <v>&lt;constant id="demo.KSDK-usb-host-cdc-serial" value="false" /&gt;</v>
+        <v>&lt;constant id="demo.KSDK-usb-host-cdc-serial" value="true" /&gt;</v>
       </c>
       <c r="G40" s="12" t="s">
         <v>69</v>
@@ -3902,7 +3920,7 @@
       <c r="AI40" s="9"/>
       <c r="AJ40" s="9"/>
     </row>
-    <row r="41" spans="3:36" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C41" s="3" t="s">
         <v>153</v>
       </c>
@@ -3965,7 +3983,7 @@
       <c r="AI41" s="9"/>
       <c r="AJ41" s="9"/>
     </row>
-    <row r="42" spans="3:36" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C42" s="3" t="s">
         <v>154</v>
       </c>
@@ -4028,7 +4046,7 @@
       <c r="AI42" s="9"/>
       <c r="AJ42" s="9"/>
     </row>
-    <row r="43" spans="3:36" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C43" s="3" t="s">
         <v>155</v>
       </c>
@@ -4091,7 +4109,7 @@
       <c r="AI43" s="9"/>
       <c r="AJ43" s="9"/>
     </row>
-    <row r="44" spans="3:36" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C44" s="3" t="s">
         <v>156</v>
       </c>
@@ -4154,7 +4172,7 @@
       <c r="AI44" s="9"/>
       <c r="AJ44" s="9"/>
     </row>
-    <row r="45" spans="3:36" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C45" s="3" t="s">
         <v>157</v>
       </c>
@@ -4217,7 +4235,7 @@
       <c r="AI45" s="9"/>
       <c r="AJ45" s="9"/>
     </row>
-    <row r="46" spans="3:36" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C46" s="3" t="s">
         <v>158</v>
       </c>
@@ -4280,7 +4298,7 @@
       <c r="AI46" s="9"/>
       <c r="AJ46" s="9"/>
     </row>
-    <row r="47" spans="3:36" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C47" s="3" t="s">
         <v>160</v>
       </c>
@@ -4333,7 +4351,7 @@
       <c r="AI47" s="9"/>
       <c r="AJ47" s="9"/>
     </row>
-    <row r="48" spans="3:36" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C48" s="3" t="s">
         <v>162</v>
       </c>
@@ -4374,7 +4392,7 @@
       <c r="AI48" s="9"/>
       <c r="AJ48" s="9"/>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.35">
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
       <c r="I49" s="12"/>
@@ -4406,7 +4424,10 @@
       <c r="AI49" s="9"/>
       <c r="AJ49" s="9"/>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="D50" s="3" t="s">
+        <v>179</v>
+      </c>
       <c r="G50" s="12"/>
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
@@ -4438,8 +4459,17 @@
       <c r="AI50" s="9"/>
       <c r="AJ50" s="9"/>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="G51" s="12"/>
+    <row r="51" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="C51" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D51" s="3" t="str">
+        <f>IF(ISBLANK(INDEX(E51:AJ51,$D$1)),"","         &lt;constant id="""&amp;C51&amp;""" value=""M&amp;KDS_DEVICE;"" /&gt;")</f>
+        <v xml:space="preserve">         &lt;constant id="usbDeviceName" value="M&amp;KDS_DEVICE;" /&gt;</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>16</v>
+      </c>
       <c r="H51" s="12"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
@@ -4470,7 +4500,10 @@
       <c r="AI51" s="9"/>
       <c r="AJ51" s="9"/>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="D52" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="G52" s="12"/>
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
@@ -4502,8 +4535,17 @@
       <c r="AI52" s="9"/>
       <c r="AJ52" s="9"/>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="G53" s="12"/>
+    <row r="53" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="C53" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D53" s="3" t="str">
+        <f>IF(ISBLANK(INDEX(E53:AJ53,$D$1)),"","         &lt;constant id="""&amp;C53&amp;"""   value=""M&amp;KDS_DEVICE;"" /&gt;")</f>
+        <v xml:space="preserve">         &lt;constant id="usbHostName"   value="M&amp;KDS_DEVICE;" /&gt;</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>16</v>
+      </c>
       <c r="H53" s="12"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
@@ -4534,7 +4576,10 @@
       <c r="AI53" s="9"/>
       <c r="AJ53" s="9"/>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="D54" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="G54" s="12"/>
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
@@ -4566,8 +4611,17 @@
       <c r="AI54" s="9"/>
       <c r="AJ54" s="9"/>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="G55" s="12"/>
+    <row r="55" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="C55" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D55" s="3" t="str">
+        <f>IF(ISBLANK(INDEX(E55:AJ55,$D$1)),"","         &lt;constant id="""&amp;C55&amp;"""    value=""M&amp;KDS_DEVICE;"" /&gt;")</f>
+        <v xml:space="preserve">         &lt;constant id="usbOtgName"    value="M&amp;KDS_DEVICE;" /&gt;</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>16</v>
+      </c>
       <c r="H55" s="12"/>
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
@@ -4598,7 +4652,7 @@
       <c r="AI55" s="9"/>
       <c r="AJ55" s="9"/>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.35">
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
       <c r="I56" s="12"/>
@@ -4630,7 +4684,7 @@
       <c r="AI56" s="9"/>
       <c r="AJ56" s="9"/>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.35">
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
       <c r="I57" s="12"/>
@@ -4662,7 +4716,7 @@
       <c r="AI57" s="9"/>
       <c r="AJ57" s="9"/>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.35">
       <c r="G58" s="12"/>
       <c r="H58" s="12"/>
       <c r="I58" s="12"/>
@@ -4694,7 +4748,7 @@
       <c r="AI58" s="9"/>
       <c r="AJ58" s="9"/>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.35">
       <c r="G59" s="12"/>
       <c r="H59" s="12"/>
       <c r="I59" s="12"/>
@@ -4726,7 +4780,7 @@
       <c r="AI59" s="9"/>
       <c r="AJ59" s="9"/>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.35">
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
       <c r="I60" s="12"/>
@@ -4758,112 +4812,41 @@
       <c r="AI60" s="9"/>
       <c r="AJ60" s="9"/>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D61" s="3" t="str">
-        <f>"&lt;constant id=""demo."&amp;C61&amp;""" value="""&amp;IF(ISBLANK(INDEX(E61:AJ61,$D$1)),"false","true")&amp;""" /&gt;"</f>
-        <v>&lt;constant id="demo.KSDK-LPTMR-comm" value="false" /&gt;</v>
-      </c>
-      <c r="E61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I61" s="16"/>
-      <c r="J61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K61" s="16"/>
-      <c r="L61" s="16"/>
-      <c r="M61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N61" s="16"/>
-      <c r="O61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="U61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="V61" s="16"/>
-      <c r="W61" s="16"/>
-      <c r="X61" s="16"/>
-      <c r="Y61" s="16"/>
-      <c r="Z61" s="16"/>
-      <c r="AA61" s="16"/>
-      <c r="AB61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD61" s="16"/>
-      <c r="AE61" s="16"/>
-      <c r="AF61" s="16"/>
-      <c r="AG61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI61" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJ61" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D62" s="3" t="str">
-        <f>"&lt;constant id=""demo."&amp;C62&amp;""" value="""&amp;IF(ISBLANK(INDEX(E62:AJ62,$D$1)),"false","true")&amp;""" /&gt;"</f>
-        <v>&lt;constant id="demo.KSDK-flextimer_pwm_demo" value="false" /&gt;</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G62" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H62" s="12" t="s">
-        <v>16</v>
-      </c>
+    <row r="61" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="12"/>
+      <c r="K61" s="12"/>
+      <c r="L61" s="12"/>
+      <c r="M61" s="12"/>
+      <c r="N61" s="12"/>
+      <c r="O61" s="12"/>
+      <c r="P61" s="13"/>
+      <c r="Q61" s="13"/>
+      <c r="R61" s="13"/>
+      <c r="S61" s="13"/>
+      <c r="T61" s="13"/>
+      <c r="U61" s="13"/>
+      <c r="V61" s="13"/>
+      <c r="W61" s="13"/>
+      <c r="X61" s="13"/>
+      <c r="Y61" s="13"/>
+      <c r="Z61" s="13"/>
+      <c r="AA61" s="13"/>
+      <c r="AB61" s="9"/>
+      <c r="AC61" s="9"/>
+      <c r="AD61" s="9"/>
+      <c r="AE61" s="9"/>
+      <c r="AF61" s="9"/>
+      <c r="AG61" s="9"/>
+      <c r="AH61" s="9"/>
+      <c r="AI61" s="9"/>
+      <c r="AJ61" s="9"/>
+    </row>
+    <row r="62" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
       <c r="I62" s="12"/>
       <c r="J62" s="12"/>
       <c r="K62" s="12"/>
@@ -4871,239 +4854,374 @@
       <c r="M62" s="12"/>
       <c r="N62" s="12"/>
       <c r="O62" s="12"/>
-      <c r="P62" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q62" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="R62" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="S62" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="T62" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="U62" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="V62" s="13" t="s">
-        <v>16</v>
-      </c>
+      <c r="P62" s="13"/>
+      <c r="Q62" s="13"/>
+      <c r="R62" s="13"/>
+      <c r="S62" s="13"/>
+      <c r="T62" s="13"/>
+      <c r="U62" s="13"/>
+      <c r="V62" s="13"/>
       <c r="W62" s="13"/>
       <c r="X62" s="13"/>
       <c r="Y62" s="13"/>
       <c r="Z62" s="13"/>
       <c r="AA62" s="13"/>
-      <c r="AB62" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC62" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="AB62" s="9"/>
+      <c r="AC62" s="9"/>
       <c r="AD62" s="9"/>
       <c r="AE62" s="9"/>
       <c r="AF62" s="9"/>
-      <c r="AG62" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH62" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI62" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJ62" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AG62" s="9"/>
+      <c r="AH62" s="9"/>
+      <c r="AI62" s="9"/>
+      <c r="AJ62" s="9"/>
+    </row>
+    <row r="63" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D63" s="3" t="str">
+        <f>"&lt;constant id=""demo."&amp;C63&amp;""" value="""&amp;IF(ISBLANK(INDEX(E63:AJ63,$D$1)),"false","true")&amp;""" /&gt;"</f>
+        <v>&lt;constant id="demo.KSDK-LPTMR-comm" value="true" /&gt;</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" s="16"/>
+      <c r="J63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K63" s="16"/>
+      <c r="L63" s="16"/>
+      <c r="M63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="N63" s="16"/>
+      <c r="O63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="P63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="R63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="S63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="T63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="U63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="V63" s="16"/>
+      <c r="W63" s="16"/>
+      <c r="X63" s="16"/>
+      <c r="Y63" s="16"/>
+      <c r="Z63" s="16"/>
+      <c r="AA63" s="16"/>
+      <c r="AB63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD63" s="16"/>
+      <c r="AE63" s="16"/>
+      <c r="AF63" s="16"/>
+      <c r="AG63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI63" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ63" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D64" s="3" t="str">
+        <f>"&lt;constant id=""demo."&amp;C64&amp;""" value="""&amp;IF(ISBLANK(INDEX(E64:AJ64,$D$1)),"false","true")&amp;""" /&gt;"</f>
+        <v>&lt;constant id="demo.KSDK-flextimer_pwm_demo" value="true" /&gt;</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H64" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12"/>
+      <c r="L64" s="12"/>
+      <c r="M64" s="12"/>
+      <c r="N64" s="12"/>
+      <c r="O64" s="12"/>
+      <c r="P64" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q64" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="R64" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="S64" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="T64" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="U64" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="V64" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="W64" s="13"/>
+      <c r="X64" s="13"/>
+      <c r="Y64" s="13"/>
+      <c r="Z64" s="13"/>
+      <c r="AA64" s="13"/>
+      <c r="AB64" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC64" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD64" s="9"/>
+      <c r="AE64" s="9"/>
+      <c r="AF64" s="9"/>
+      <c r="AG64" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH64" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI64" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ64" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B65" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="3" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="3" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="3" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="3" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="3" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" s="3" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="3" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="3" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="3" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="3" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="3" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="3" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="3" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="3" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" s="3" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="3" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="3" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="3" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" s="3" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="3" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" s="3" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="3" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="3" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" s="3" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" s="3" t="s">
         <v>138</v>
       </c>
     </row>
@@ -5145,12 +5263,12 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" customWidth="1"/>
+    <col min="1" max="1" width="39.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="69.599999999999994" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="70.5" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>36</v>
       </c>
@@ -5215,7 +5333,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>145</v>
       </c>
@@ -5226,7 +5344,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>146</v>
       </c>
@@ -5237,7 +5355,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>147</v>
       </c>
@@ -5245,7 +5363,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>148</v>
       </c>
@@ -5253,7 +5371,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>149</v>
       </c>
@@ -5261,7 +5379,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>150</v>
       </c>
@@ -5269,7 +5387,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>151</v>
       </c>
@@ -5277,7 +5395,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>159</v>
       </c>
@@ -5285,7 +5403,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>152</v>
       </c>
@@ -5293,7 +5411,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>153</v>
       </c>
@@ -5301,7 +5419,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>154</v>
       </c>
@@ -5309,7 +5427,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>155</v>
       </c>
@@ -5317,7 +5435,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>156</v>
       </c>
@@ -5325,7 +5443,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>157</v>
       </c>
@@ -5333,7 +5451,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>158</v>
       </c>
@@ -5341,37 +5459,37 @@
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="B20" s="17" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="B21" s="17" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="B22" s="17" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="B23" s="17" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="B24" s="17" t="s">
         <v>173</v>
       </c>

</xml_diff>